<commit_message>
Modified product price retrieval function
</commit_message>
<xml_diff>
--- a/Test/bin/testData/TestData.xlsx
+++ b/Test/bin/testData/TestData.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="4035" windowWidth="11340" xWindow="0" yWindow="2520"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="10575" windowHeight="3570"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
   <oleSize ref="A1"/>
@@ -17,28 +17,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Amazon Product Name</t>
-  </si>
-  <si>
-    <t>Amazon Price</t>
-  </si>
-  <si>
-    <t>Flipkart Product Price</t>
-  </si>
-  <si>
-    <t>Flipkart Price</t>
-  </si>
-  <si>
-    <t>Sony 80 cm (32 inches) Bravia KLV-32W512D HD Ready Smart LED TV</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -56,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -64,36 +47,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -102,10 +67,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -261,7 +226,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -270,13 +235,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -286,7 +251,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -295,7 +260,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -304,7 +269,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -314,12 +279,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -350,7 +315,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -369,7 +334,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -382,41 +347,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="42.7109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="1" width="13.140625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="1" width="37.42578125" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.5703125" collapsed="false"/>
+    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
@@ -429,7 +374,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -441,6 +386,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>